<commit_message>
LJ interface program completed to initial levels
</commit_message>
<xml_diff>
--- a/0_AvionicsnDAQ/Datalogger/AIN_Scaling.xlsx
+++ b/0_AvionicsnDAQ/Datalogger/AIN_Scaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\LADS-GIT-Repos\0_AvionicsnDAQ\Datalogger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA3B125-F70D-4E95-9B3C-0701F1956A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2019DC3A-4FA0-4752-BED5-3F7B8E63E1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8730" yWindow="2130" windowWidth="21600" windowHeight="11295" xr2:uid="{EAA209E0-C57D-4233-A22F-F3EB3D772D77}"/>
+    <workbookView xWindow="-20970" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{EAA209E0-C57D-4233-A22F-F3EB3D772D77}"/>
   </bookViews>
   <sheets>
     <sheet name="Scaling" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -559,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I17">
         <v>0</v>

</xml_diff>